<commit_message>
received updated file name from sequencing center
</commit_message>
<xml_diff>
--- a/fastqFiles/fastq_01.22.21.xlsx
+++ b/fastqFiles/fastq_01.22.21.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/fastqFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BFD98A8B-B655-0540-BCC4-6F0A95B20B03}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E0C1B2-D28A-E749-973C-33ADA49FDC01}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4780" yWindow="460" windowWidth="27640" windowHeight="16940" xr2:uid="{4D567BF4-64D3-674A-B386-88589DAC0A18}"/>
+    <workbookView xWindow="11760" yWindow="460" windowWidth="27640" windowHeight="16940" xr2:uid="{4D567BF4-64D3-674A-B386-88589DAC0A18}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -78,218 +78,224 @@
     <t>fullRNASeq</t>
   </si>
   <si>
-    <t>Brent_2e_1_GTAC_1_SIC_Index2_06_TGAGGTT_GACCTTGT</t>
-  </si>
-  <si>
-    <t>Brent_2e_2_GTAC_2_SIC_Index2_06_GCTTAGA_GACCTTGT</t>
-  </si>
-  <si>
-    <t>Brent_2e_3_GTAC_3_SIC_Index2_06_ATGACAG_GACCTTGT</t>
-  </si>
-  <si>
-    <t>Brent_2e_4_GTAC_4_SIC_Index2_06_CACCTCC_GACCTTGT</t>
-  </si>
-  <si>
-    <t>Brent_2e_5_GTAC_5_SIC_Index2_06_ATCGAGC_GACCTTGT</t>
-  </si>
-  <si>
-    <t>Brent_2e_6_GTAC_6_SIC_Index2_06_TACTCTA_GACCTTGT</t>
-  </si>
-  <si>
-    <t>Brent_2e_7_GTAC_7_SIC_Index2_06_AGACTGA_GACCTTGT</t>
-  </si>
-  <si>
-    <t>Brent_2e_8_GTAC_8_SIC_Index2_06_CTTGGAA_GACCTTGT</t>
-  </si>
-  <si>
-    <t>Brent_2e_9_GTAC_9_SIC_Index2_06_CCGATTA_GACCTTGT</t>
-  </si>
-  <si>
-    <t>Brent_2e_10_GTAC_10_SIC_Index2_06_GGCAGCG_GACCTTGT</t>
-  </si>
-  <si>
-    <t>Brent_2e_11_GTAC_11_SIC_Index2_06_CCATCAT_GACCTTGT</t>
-  </si>
-  <si>
-    <t>Brent_2e_12_GTAC_12_SIC_Index2_06_TAACAAG_GACCTTGT</t>
-  </si>
-  <si>
-    <t>Brent_2e_13_GTAC_13_SIC_Index2_06_GAGGCGT_GACCTTGT</t>
-  </si>
-  <si>
-    <t>Brent_2e_14_GTAC_14_SIC_Index2_06_TTTAACT_GACCTTGT</t>
-  </si>
-  <si>
-    <t>Brent_2e_15_GTAC_15_SIC_Index2_06_GGTCCTC_GACCTTGT</t>
-  </si>
-  <si>
-    <t>Brent_2e_16_GTAC_16_SIC_Index2_06_CGGTGGC_GACCTTGT</t>
-  </si>
-  <si>
-    <t>Brent_2e_17_GTAC_17_SIC_Index2_06_ACTGTCG_GACCTTGT</t>
-  </si>
-  <si>
-    <t>Brent_2e_18_GTAC_18_SIC_Index2_06_GTATTTG_GACCTTGT</t>
-  </si>
-  <si>
-    <t>Brent_2e_19_GTAC_19_SIC_Index2_06_GAGTACG_GACCTTGT</t>
-  </si>
-  <si>
-    <t>Brent_2e_20_GTAC_20_SIC_Index2_06_ACAGATA_GACCTTGT</t>
-  </si>
-  <si>
-    <t>Brent_2e_21_GTAC_21_SIC_Index2_06_CTCAATG_GACCTTGT</t>
-  </si>
-  <si>
-    <t>Brent_2e_22_GTAC_22_SIC_Index2_06_AAATGCA_GACCTTGT</t>
-  </si>
-  <si>
-    <t>Brent_2e_23_GTAC_23_SIC_Index2_06_ACGCGGG_GACCTTGT</t>
-  </si>
-  <si>
-    <t>Brent_2e_24_GTAC_24_SIC_Index2_06_GGAGTCC_GACCTTGT</t>
-  </si>
-  <si>
-    <t>Brent_2e_25_GTAC_25_SIC_Index2_06_CGTCGCT_GACCTTGT</t>
-  </si>
-  <si>
-    <t>Brent_2e_26_GTAC_26_SIC_Index2_06_TCAACTG_GACCTTGT</t>
-  </si>
-  <si>
     <t>01.09.21</t>
   </si>
   <si>
-    <t>Brent_DA_19_GTAC_1_SIC_Index2_10_TGAGGTT_GCTTCTGT</t>
-  </si>
-  <si>
-    <t>Brent_DA_20_GTAC_2_SIC_Index2_10_GCTTAGA_GCTTCTGT</t>
-  </si>
-  <si>
-    <t>Brent_DA_21_GTAC_3_SIC_Index2_10_ATGACAG_GCTTCTGT</t>
-  </si>
-  <si>
-    <t>Brent_DA_22_GTAC_4_SIC_Index2_10_CACCTCC_GCTTCTGT</t>
-  </si>
-  <si>
-    <t>Brent_DA_23_GTAC_5_SIC_Index2_10_ATCGAGC_GCTTCTGT</t>
-  </si>
-  <si>
-    <t>Brent_DA_24_GTAC_6_SIC_Index2_10_TACTCTA_GCTTCTGT</t>
-  </si>
-  <si>
-    <t>Brent_DA_25_GTAC_7_SIC_Index2_10_AGACTGA_GCTTCTGT</t>
-  </si>
-  <si>
-    <t>Brent_DA_26_GTAC_8_SIC_Index2_10_CTTGGAA_GCTTCTGT</t>
-  </si>
-  <si>
-    <t>Brent_DA_27_GTAC_9_SIC_Index2_10_CCGATTA_GCTTCTGT</t>
-  </si>
-  <si>
-    <t>Brent_DA_28_GTAC_10_SIC_Index2_10_GGCAGCG_GCTTCTGT</t>
-  </si>
-  <si>
-    <t>Brent_DA_29_GTAC_11_SIC_Index2_10_CCATCAT_GCTTCTGT</t>
-  </si>
-  <si>
-    <t>Brent_DA_30_GTAC_12_SIC_Index2_10_TAACAAG_GCTTCTGT</t>
-  </si>
-  <si>
-    <t>Brent_DA_31_GTAC_13_SIC_Index2_10_GAGGCGT_GCTTCTGT</t>
-  </si>
-  <si>
-    <t>Brent_DA_32_GTAC_14_SIC_Index2_10_TTTAACT_GCTTCTGT</t>
-  </si>
-  <si>
-    <t>Brent_DA_33_GTAC_15_SIC_Index2_10_GGTCCTC_GCTTCTGT</t>
-  </si>
-  <si>
-    <t>Brent_DA_34_GTAC_16_SIC_Index2_10_CGGTGGC_GCTTCTGT</t>
-  </si>
-  <si>
-    <t>Brent_DA_35_GTAC_17_SIC_Index2_10_ACTGTCG_GCTTCTGT</t>
-  </si>
-  <si>
-    <t>Brent_DA_36_GTAC_18_SIC_Index2_10_GTATTTG_GCTTCTGT</t>
-  </si>
-  <si>
-    <t>Brent_DA_37_GTAC_19_SIC_Index2_10_GAGTACG_GCTTCTGT</t>
-  </si>
-  <si>
-    <t>Brent_DA_38_GTAC_20_SIC_Index2_10_ACAGATA_GCTTCTGT</t>
-  </si>
-  <si>
-    <t>Brent_DA_39_GTAC_21_SIC_Index2_10_CTCAATG_GCTTCTGT</t>
-  </si>
-  <si>
-    <t>Brent_DA_40_GTAC_22_SIC_Index2_10_AAATGCA_GCTTCTGT</t>
-  </si>
-  <si>
-    <t>Brent_DA_41_GTAC_23_SIC_Index2_10_ACGCGGG_GCTTCTGT</t>
-  </si>
-  <si>
-    <t>Brent_DA_42_GTAC_24_SIC_Index2_10_GGAGTCC_GCTTCTGT</t>
-  </si>
-  <si>
-    <t>Brent_DA_43_GTAC_25_SIC_Index2_10_CGTCGCT_GCTTCTGT</t>
-  </si>
-  <si>
-    <t>Brent_DA_44_GTAC_26_SIC_Index2_10_TCAACTG_GCTTCTGT</t>
-  </si>
-  <si>
-    <t>Brent_DA_45_GTAC_27_SIC_Index2_10_TGTTTGT_GCTTCTGT</t>
-  </si>
-  <si>
-    <t>Brent_DA_46_GTAC_28_SIC_Index2_10_TACATGG_GCTTCTGT</t>
-  </si>
-  <si>
-    <t>Brent_DA_47_GTAC_29_SIC_Index2_10_GTTCTCA_GCTTCTGT</t>
-  </si>
-  <si>
-    <t>Brent_DA_48_GTAC_30_SIC_Index2_10_CTGGTGG_GCTTCTGT</t>
-  </si>
-  <si>
-    <t>Brent_DA_49_GTAC_31_SIC_Index2_10_TGCCCAT_GCTTCTGT</t>
-  </si>
-  <si>
-    <t>Brent_DA_50_GTAC_32_SIC_Index2_10_AAACCTT_GCTTCTGT</t>
-  </si>
-  <si>
-    <t>Brent_DA_51_GTAC_33_SIC_Index2_10_ACCATAC_GCTTCTGT</t>
-  </si>
-  <si>
-    <t>Brent_DA_52_GTAC_41_SIC_Index2_10_TTGCCCC_GCTTCTGT</t>
-  </si>
-  <si>
-    <t>Brent_DA_53_GTAC_42_SIC_Index2_10_ACTCCAA_GCTTCTGT</t>
-  </si>
-  <si>
-    <t>Brent_DA_54_GTAC_43_SIC_Index2_10_TGTGCCA_GCTTCTGT</t>
-  </si>
-  <si>
-    <t>Brent_DA_55_GTAC_37_SIC_Index2_10_TTTTGTC_GCTTCTGT</t>
-  </si>
-  <si>
-    <t>Brent_DA_56_GTAC_38_SIC_Index2_10_ACCCACT_GCTTCTGT</t>
-  </si>
-  <si>
-    <t>Brent_DA_57_GTAC_39_SIC_Index2_10_CCGGACC_GCTTCTGT</t>
-  </si>
-  <si>
-    <t>Brent_DA_58_GTAC_40_SIC_Index2_10_GTACGGC_GCTTCTGT</t>
+    <t>Brent_2e_2_GTAC_2_SIC_Index2_06_GCTTAGA_GACCTTGT_S43_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2e_3_GTAC_3_SIC_Index2_06_ATGACAG_GACCTTGT_S44_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2e_4_GTAC_4_SIC_Index2_06_CACCTCC_GACCTTGT_S45_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2e_5_GTAC_5_SIC_Index2_06_ATCGAGC_GACCTTGT_S46_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2e_1_GTAC_1_SIC_Index2_06_TGAGGTT_GACCTTGT_S42_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2e_6_GTAC_6_SIC_Index2_06_TACTCTA_GACCTTGT_S47_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2e_7_GTAC_7_SIC_Index2_06_AGACTGA_GACCTTGT_S48_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2e_8_GTAC_8_SIC_Index2_06_CTTGGAA_GACCTTGT_S49_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2e_9_GTAC_9_SIC_Index2_06_CCGATTA_GACCTTGT_S50_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2e_10_GTAC_10_SIC_Index2_06_GGCAGCG_GACCTTGT_S51_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2e_11_GTAC_11_SIC_Index2_06_CCATCAT_GACCTTGT_S52_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2e_12_GTAC_12_SIC_Index2_06_TAACAAG_GACCTTGT_S53_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2e_13_GTAC_13_SIC_Index2_06_GAGGCGT_GACCTTGT_S54_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2e_14_GTAC_14_SIC_Index2_06_TTTAACT_GACCTTGT_S55_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2e_15_GTAC_15_SIC_Index2_06_GGTCCTC_GACCTTGT_S56_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2e_16_GTAC_16_SIC_Index2_06_CGGTGGC_GACCTTGT_S57_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2e_17_GTAC_17_SIC_Index2_06_ACTGTCG_GACCTTGT_S58_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2e_18_GTAC_18_SIC_Index2_06_GTATTTG_GACCTTGT_S59_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2e_19_GTAC_19_SIC_Index2_06_GAGTACG_GACCTTGT_S60_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2e_20_GTAC_20_SIC_Index2_06_ACAGATA_GACCTTGT_S61_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2e_21_GTAC_21_SIC_Index2_06_CTCAATG_GACCTTGT_S62_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2e_22_GTAC_22_SIC_Index2_06_AAATGCA_GACCTTGT_S63_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2e_23_GTAC_23_SIC_Index2_06_ACGCGGG_GACCTTGT_S64_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2e_24_GTAC_24_SIC_Index2_06_GGAGTCC_GACCTTGT_S65_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2e_25_GTAC_25_SIC_Index2_06_CGTCGCT_GACCTTGT_S66_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2e_26_GTAC_26_SIC_Index2_06_TCAACTG_GACCTTGT_S67_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_19_GTAC_1_SIC_Index2_10_TGAGGTT_GCTTCTGT_S2_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_20_GTAC_2_SIC_Index2_10_GCTTAGA_GCTTCTGT_S3_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_21_GTAC_3_SIC_Index2_10_ATGACAG_GCTTCTGT_S4_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_22_GTAC_4_SIC_Index2_10_CACCTCC_GCTTCTGT_S5_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_23_GTAC_5_SIC_Index2_10_ATCGAGC_GCTTCTGT_S6_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_24_GTAC_6_SIC_Index2_10_TACTCTA_GCTTCTGT_S7_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_25_GTAC_7_SIC_Index2_10_AGACTGA_GCTTCTGT_S8_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_26_GTAC_8_SIC_Index2_10_CTTGGAA_GCTTCTGT_S9_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_27_GTAC_9_SIC_Index2_10_CCGATTA_GCTTCTGT_S10_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_28_GTAC_10_SIC_Index2_10_GGCAGCG_GCTTCTGT_S11_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_29_GTAC_11_SIC_Index2_10_CCATCAT_GCTTCTGT_S12_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_30_GTAC_12_SIC_Index2_10_TAACAAG_GCTTCTGT_S13_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_31_GTAC_13_SIC_Index2_10_GAGGCGT_GCTTCTGT_S14_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_32_GTAC_14_SIC_Index2_10_TTTAACT_GCTTCTGT_S15_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_33_GTAC_15_SIC_Index2_10_GGTCCTC_GCTTCTGT_S16_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_34_GTAC_16_SIC_Index2_10_CGGTGGC_GCTTCTGT_S17_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_35_GTAC_17_SIC_Index2_10_ACTGTCG_GCTTCTGT_S18_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_36_GTAC_18_SIC_Index2_10_GTATTTG_GCTTCTGT_S19_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_37_GTAC_19_SIC_Index2_10_GAGTACG_GCTTCTGT_S20_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_38_GTAC_20_SIC_Index2_10_ACAGATA_GCTTCTGT_S21_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_39_GTAC_21_SIC_Index2_10_CTCAATG_GCTTCTGT_S22_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_40_GTAC_22_SIC_Index2_10_AAATGCA_GCTTCTGT_S23_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_41_GTAC_23_SIC_Index2_10_ACGCGGG_GCTTCTGT_S24_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_42_GTAC_24_SIC_Index2_10_GGAGTCC_GCTTCTGT_S25_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_43_GTAC_25_SIC_Index2_10_CGTCGCT_GCTTCTGT_S26_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_44_GTAC_26_SIC_Index2_10_TCAACTG_GCTTCTGT_S27_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_45_GTAC_27_SIC_Index2_10_TGTTTGT_GCTTCTGT_S28_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_46_GTAC_28_SIC_Index2_10_TACATGG_GCTTCTGT_S29_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_47_GTAC_29_SIC_Index2_10_GTTCTCA_GCTTCTGT_S30_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_48_GTAC_30_SIC_Index2_10_CTGGTGG_GCTTCTGT_S31_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_49_GTAC_31_SIC_Index2_10_TGCCCAT_GCTTCTGT_S32_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_50_GTAC_32_SIC_Index2_10_AAACCTT_GCTTCTGT_S33_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_51_GTAC_33_SIC_Index2_10_ACCATAC_GCTTCTGT_S34_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_52_GTAC_41_SIC_Index2_10_TTGCCCC_GCTTCTGT_S35_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_53_GTAC_42_SIC_Index2_10_ACTCCAA_GCTTCTGT_S36_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_54_GTAC_43_SIC_Index2_10_TGTGCCA_GCTTCTGT_S37_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_55_GTAC_37_SIC_Index2_10_TTTTGTC_GCTTCTGT_S38_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_56_GTAC_38_SIC_Index2_10_ACCCACT_GCTTCTGT_S39_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_57_GTAC_39_SIC_Index2_10_CCGGACC_GCTTCTGT_S40_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_58_GTAC_40_SIC_Index2_10_GTACGGC_GCTTCTGT_S41_R1_001.fastq.gz</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8.5"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -312,8 +318,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -630,11 +637,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{180FD35D-5CB7-5B4A-A003-589EE4E20EA2}">
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R17" sqref="R17"/>
+    <sheetView tabSelected="1" topLeftCell="D40" workbookViewId="0">
+      <selection activeCell="L68" sqref="L68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="11" width="10.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -705,8 +715,8 @@
       <c r="K2">
         <v>2985944</v>
       </c>
-      <c r="L2" t="s">
-        <v>17</v>
+      <c r="L2" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -740,7 +750,7 @@
       <c r="K3">
         <v>1760291</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -775,7 +785,7 @@
       <c r="K4">
         <v>2963867</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -810,7 +820,7 @@
       <c r="K5">
         <v>1573770</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -845,7 +855,7 @@
       <c r="K6">
         <v>981224</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L6" s="1" t="s">
         <v>21</v>
       </c>
     </row>
@@ -880,8 +890,8 @@
       <c r="K7">
         <v>1272131</v>
       </c>
-      <c r="L7" t="s">
-        <v>22</v>
+      <c r="L7" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -915,8 +925,8 @@
       <c r="K8">
         <v>2784298</v>
       </c>
-      <c r="L8" t="s">
-        <v>23</v>
+      <c r="L8" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -950,8 +960,8 @@
       <c r="K9">
         <v>2784687</v>
       </c>
-      <c r="L9" t="s">
-        <v>24</v>
+      <c r="L9" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -985,8 +995,8 @@
       <c r="K10">
         <v>35127909</v>
       </c>
-      <c r="L10" t="s">
-        <v>25</v>
+      <c r="L10" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
@@ -1020,8 +1030,8 @@
       <c r="K11">
         <v>34103079</v>
       </c>
-      <c r="L11" t="s">
-        <v>26</v>
+      <c r="L11" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -1055,8 +1065,8 @@
       <c r="K12">
         <v>28612543</v>
       </c>
-      <c r="L12" t="s">
-        <v>27</v>
+      <c r="L12" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
@@ -1090,8 +1100,8 @@
       <c r="K13">
         <v>7643920</v>
       </c>
-      <c r="L13" t="s">
-        <v>28</v>
+      <c r="L13" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
@@ -1125,8 +1135,8 @@
       <c r="K14">
         <v>12135264</v>
       </c>
-      <c r="L14" t="s">
-        <v>29</v>
+      <c r="L14" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
@@ -1160,8 +1170,8 @@
       <c r="K15">
         <v>5549230</v>
       </c>
-      <c r="L15" t="s">
-        <v>30</v>
+      <c r="L15" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
@@ -1195,8 +1205,8 @@
       <c r="K16">
         <v>8117805</v>
       </c>
-      <c r="L16" t="s">
-        <v>31</v>
+      <c r="L16" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
@@ -1230,8 +1240,8 @@
       <c r="K17">
         <v>3333589</v>
       </c>
-      <c r="L17" t="s">
-        <v>32</v>
+      <c r="L17" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
@@ -1265,8 +1275,8 @@
       <c r="K18">
         <v>6520182</v>
       </c>
-      <c r="L18" t="s">
-        <v>33</v>
+      <c r="L18" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
@@ -1300,8 +1310,8 @@
       <c r="K19">
         <v>7828772</v>
       </c>
-      <c r="L19" t="s">
-        <v>34</v>
+      <c r="L19" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
@@ -1335,8 +1345,8 @@
       <c r="K20">
         <v>8342075</v>
       </c>
-      <c r="L20" t="s">
-        <v>35</v>
+      <c r="L20" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
@@ -1370,8 +1380,8 @@
       <c r="K21">
         <v>7875259</v>
       </c>
-      <c r="L21" t="s">
-        <v>36</v>
+      <c r="L21" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
@@ -1405,8 +1415,8 @@
       <c r="K22">
         <v>3106760</v>
       </c>
-      <c r="L22" t="s">
-        <v>37</v>
+      <c r="L22" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
@@ -1440,8 +1450,8 @@
       <c r="K23">
         <v>1374619</v>
       </c>
-      <c r="L23" t="s">
-        <v>38</v>
+      <c r="L23" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
@@ -1475,8 +1485,8 @@
       <c r="K24">
         <v>3144093</v>
       </c>
-      <c r="L24" t="s">
-        <v>39</v>
+      <c r="L24" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
@@ -1510,8 +1520,8 @@
       <c r="K25">
         <v>2911065</v>
       </c>
-      <c r="L25" t="s">
-        <v>40</v>
+      <c r="L25" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
@@ -1545,8 +1555,8 @@
       <c r="K26">
         <v>3139132</v>
       </c>
-      <c r="L26" t="s">
-        <v>41</v>
+      <c r="L26" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
@@ -1580,13 +1590,13 @@
       <c r="K27">
         <v>3202503</v>
       </c>
-      <c r="L27" t="s">
-        <v>42</v>
+      <c r="L27" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B28" t="s">
         <v>13</v>
@@ -1615,13 +1625,13 @@
       <c r="K28">
         <v>72887955</v>
       </c>
-      <c r="L28" t="s">
+      <c r="L28" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B29" t="s">
         <v>13</v>
@@ -1650,13 +1660,13 @@
       <c r="K29">
         <v>7548520</v>
       </c>
-      <c r="L29" t="s">
+      <c r="L29" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B30" t="s">
         <v>13</v>
@@ -1685,13 +1695,13 @@
       <c r="K30">
         <v>5411448</v>
       </c>
-      <c r="L30" t="s">
+      <c r="L30" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B31" t="s">
         <v>13</v>
@@ -1720,13 +1730,13 @@
       <c r="K31">
         <v>10056340</v>
       </c>
-      <c r="L31" t="s">
+      <c r="L31" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B32" t="s">
         <v>13</v>
@@ -1755,13 +1765,13 @@
       <c r="K32">
         <v>7852016</v>
       </c>
-      <c r="L32" t="s">
+      <c r="L32" s="1" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B33" t="s">
         <v>13</v>
@@ -1790,13 +1800,13 @@
       <c r="K33">
         <v>9742380</v>
       </c>
-      <c r="L33" t="s">
+      <c r="L33" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B34" t="s">
         <v>13</v>
@@ -1825,13 +1835,13 @@
       <c r="K34">
         <v>9635620</v>
       </c>
-      <c r="L34" t="s">
+      <c r="L34" s="1" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B35" t="s">
         <v>13</v>
@@ -1860,13 +1870,13 @@
       <c r="K35">
         <v>8513753</v>
       </c>
-      <c r="L35" t="s">
+      <c r="L35" s="1" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B36" t="s">
         <v>13</v>
@@ -1895,13 +1905,13 @@
       <c r="K36">
         <v>10533361</v>
       </c>
-      <c r="L36" t="s">
+      <c r="L36" s="1" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B37" t="s">
         <v>13</v>
@@ -1930,13 +1940,13 @@
       <c r="K37">
         <v>7938657</v>
       </c>
-      <c r="L37" t="s">
+      <c r="L37" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B38" t="s">
         <v>13</v>
@@ -1965,13 +1975,13 @@
       <c r="K38">
         <v>7000186</v>
       </c>
-      <c r="L38" t="s">
+      <c r="L38" s="1" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B39" t="s">
         <v>13</v>
@@ -2000,13 +2010,13 @@
       <c r="K39">
         <v>6379818</v>
       </c>
-      <c r="L39" t="s">
+      <c r="L39" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B40" t="s">
         <v>13</v>
@@ -2035,13 +2045,13 @@
       <c r="K40">
         <v>7214825</v>
       </c>
-      <c r="L40" t="s">
+      <c r="L40" s="1" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B41" t="s">
         <v>13</v>
@@ -2070,13 +2080,13 @@
       <c r="K41">
         <v>6523475</v>
       </c>
-      <c r="L41" t="s">
+      <c r="L41" s="1" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B42" t="s">
         <v>13</v>
@@ -2105,13 +2115,13 @@
       <c r="K42">
         <v>6909552</v>
       </c>
-      <c r="L42" t="s">
+      <c r="L42" s="1" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B43" t="s">
         <v>13</v>
@@ -2140,13 +2150,13 @@
       <c r="K43">
         <v>5875488</v>
       </c>
-      <c r="L43" t="s">
+      <c r="L43" s="1" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B44" t="s">
         <v>13</v>
@@ -2175,13 +2185,13 @@
       <c r="K44">
         <v>6802869</v>
       </c>
-      <c r="L44" t="s">
+      <c r="L44" s="1" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B45" t="s">
         <v>13</v>
@@ -2210,13 +2220,13 @@
       <c r="K45">
         <v>8560636</v>
       </c>
-      <c r="L45" t="s">
+      <c r="L45" s="1" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B46" t="s">
         <v>13</v>
@@ -2245,13 +2255,13 @@
       <c r="K46">
         <v>7794753</v>
       </c>
-      <c r="L46" t="s">
+      <c r="L46" s="1" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B47" t="s">
         <v>13</v>
@@ -2280,13 +2290,13 @@
       <c r="K47">
         <v>8215062</v>
       </c>
-      <c r="L47" t="s">
+      <c r="L47" s="1" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B48" t="s">
         <v>13</v>
@@ -2315,13 +2325,13 @@
       <c r="K48">
         <v>772442</v>
       </c>
-      <c r="L48" t="s">
+      <c r="L48" s="1" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B49" t="s">
         <v>13</v>
@@ -2350,13 +2360,13 @@
       <c r="K49">
         <v>5541996</v>
       </c>
-      <c r="L49" t="s">
+      <c r="L49" s="1" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B50" t="s">
         <v>13</v>
@@ -2385,13 +2395,13 @@
       <c r="K50">
         <v>6833427</v>
       </c>
-      <c r="L50" t="s">
+      <c r="L50" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B51" t="s">
         <v>13</v>
@@ -2420,13 +2430,13 @@
       <c r="K51">
         <v>6298723</v>
       </c>
-      <c r="L51" t="s">
+      <c r="L51" s="1" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B52" t="s">
         <v>13</v>
@@ -2455,13 +2465,13 @@
       <c r="K52">
         <v>5639193</v>
       </c>
-      <c r="L52" t="s">
+      <c r="L52" s="1" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B53" t="s">
         <v>13</v>
@@ -2490,13 +2500,13 @@
       <c r="K53">
         <v>8019749</v>
       </c>
-      <c r="L53" t="s">
+      <c r="L53" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B54" t="s">
         <v>13</v>
@@ -2525,13 +2535,13 @@
       <c r="K54">
         <v>6436480</v>
       </c>
-      <c r="L54" t="s">
+      <c r="L54" s="1" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B55" t="s">
         <v>13</v>
@@ -2560,13 +2570,13 @@
       <c r="K55">
         <v>6019015</v>
       </c>
-      <c r="L55" t="s">
+      <c r="L55" s="1" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B56" t="s">
         <v>13</v>
@@ -2595,13 +2605,13 @@
       <c r="K56">
         <v>6732759</v>
       </c>
-      <c r="L56" t="s">
+      <c r="L56" s="1" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B57" t="s">
         <v>13</v>
@@ -2630,13 +2640,13 @@
       <c r="K57">
         <v>7019141</v>
       </c>
-      <c r="L57" t="s">
+      <c r="L57" s="1" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B58" t="s">
         <v>13</v>
@@ -2665,13 +2675,13 @@
       <c r="K58">
         <v>6470022</v>
       </c>
-      <c r="L58" t="s">
+      <c r="L58" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B59" t="s">
         <v>13</v>
@@ -2700,13 +2710,13 @@
       <c r="K59">
         <v>5764227</v>
       </c>
-      <c r="L59" t="s">
+      <c r="L59" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B60" t="s">
         <v>13</v>
@@ -2735,13 +2745,13 @@
       <c r="K60">
         <v>7821487</v>
       </c>
-      <c r="L60" t="s">
+      <c r="L60" s="1" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B61" t="s">
         <v>13</v>
@@ -2770,13 +2780,13 @@
       <c r="K61">
         <v>6183913</v>
       </c>
-      <c r="L61" t="s">
+      <c r="L61" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B62" t="s">
         <v>13</v>
@@ -2805,13 +2815,13 @@
       <c r="K62">
         <v>7021804</v>
       </c>
-      <c r="L62" t="s">
+      <c r="L62" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B63" t="s">
         <v>13</v>
@@ -2840,13 +2850,13 @@
       <c r="K63">
         <v>6292494</v>
       </c>
-      <c r="L63" t="s">
+      <c r="L63" s="1" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B64" t="s">
         <v>13</v>
@@ -2875,13 +2885,13 @@
       <c r="K64">
         <v>6795386</v>
       </c>
-      <c r="L64" t="s">
+      <c r="L64" s="1" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B65" t="s">
         <v>13</v>
@@ -2910,13 +2920,13 @@
       <c r="K65">
         <v>6898270</v>
       </c>
-      <c r="L65" t="s">
+      <c r="L65" s="1" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B66" t="s">
         <v>13</v>
@@ -2945,13 +2955,13 @@
       <c r="K66">
         <v>6283060</v>
       </c>
-      <c r="L66" t="s">
+      <c r="L66" s="1" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B67" t="s">
         <v>13</v>
@@ -2980,7 +2990,7 @@
       <c r="K67">
         <v>5078782</v>
       </c>
-      <c r="L67" t="s">
+      <c r="L67" s="1" t="s">
         <v>83</v>
       </c>
     </row>

</xml_diff>